<commit_message>
Actualizacion miercoles 12 de mayo
</commit_message>
<xml_diff>
--- a/info excel/REGISTRO PERSONAL SERVICIOS PCR.xlsx
+++ b/info excel/REGISTRO PERSONAL SERVICIOS PCR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56961\Desktop\Heavy Duty\info excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1014834-6E52-4CAB-B125-B13EAD25F796}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B6678B-91E1-45B2-8747-8DED5377F3BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{0D2AEC7C-D87E-4142-A96E-B946B04B6E1C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="572">
   <si>
     <t>NOMBRE</t>
   </si>
@@ -2027,9 +2027,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2047,6 +2044,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares [0]" xfId="1" builtinId="6"/>
@@ -2475,15 +2475,15 @@
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="35"/>
+      <c r="E1" s="44"/>
       <c r="F1" s="8"/>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="35"/>
+      <c r="H1" s="44"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
       <c r="K1" s="6"/>
@@ -6520,8 +6520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D99D70D-18BB-4572-89FC-6F293C4FC3E4}">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6581,185 +6581,191 @@
         <v>495</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="37" t="str">
+    <row r="2" spans="1:15" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="43" t="s">
+        <v>571</v>
+      </c>
+      <c r="B2" s="36" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna1]])</f>
         <v>ALAN ANDRES</v>
       </c>
-      <c r="C2" s="36" t="str">
+      <c r="C2" s="35" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna2]])</f>
         <v>ESPINOZA ACEVEDO</v>
       </c>
-      <c r="D2" s="36" t="str">
+      <c r="D2" s="35" t="str">
         <f>B2&amp;" " &amp;C2</f>
         <v>ALAN ANDRES ESPINOZA ACEVEDO</v>
       </c>
-      <c r="E2" s="36" t="str">
+      <c r="E2" s="35" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna3]])</f>
         <v>JEFE DE EQUIPO DE MANTENCION</v>
       </c>
-      <c r="F2" s="38" t="str">
+      <c r="F2" s="37" t="str">
         <f>UPPER(Tabla1[[#This Row],[NOMBRE COMPLETO]])</f>
         <v/>
       </c>
-      <c r="G2" s="38" t="str">
+      <c r="G2" s="37" t="str">
         <f>UPPER(Tabla1[[#This Row],[CARGO ACTUAL]])</f>
         <v/>
       </c>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39" t="str">
+      <c r="H2" s="38"/>
+      <c r="I2" s="38" t="str">
         <f>UPPER(Tabla1[[#This Row],[EXPERIENCIA EN EL RUBRO (AÑO Y MES DE PRIMER TRABAJO EN EL RUBRO DE GRUAS TORRE)]])</f>
         <v/>
       </c>
-      <c r="J2" s="40"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="41"/>
-    </row>
-    <row r="3" spans="1:15" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="37" t="str">
+      <c r="J2" s="39"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="40"/>
+    </row>
+    <row r="3" spans="1:15" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="36" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna1]])</f>
         <v xml:space="preserve">ALEJANDRO </v>
       </c>
-      <c r="C3" s="36" t="str">
+      <c r="C3" s="35" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna2]])</f>
         <v>GONZALEZ LOPEZ</v>
       </c>
-      <c r="D3" s="36" t="str">
+      <c r="D3" s="35" t="str">
         <f t="shared" ref="D3:D4" si="0">B3&amp;" " &amp;C3</f>
         <v>ALEJANDRO  GONZALEZ LOPEZ</v>
       </c>
-      <c r="E3" s="36" t="str">
+      <c r="E3" s="35" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna3]])</f>
         <v>JEFE MONTAJE PC</v>
       </c>
-      <c r="F3" s="38" t="str">
+      <c r="F3" s="37" t="str">
         <f>UPPER(Tabla1[[#This Row],[NOMBRE COMPLETO]])</f>
         <v/>
       </c>
-      <c r="G3" s="38" t="str">
+      <c r="G3" s="37" t="str">
         <f>UPPER(Tabla1[[#This Row],[CARGO ACTUAL]])</f>
         <v/>
       </c>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="41"/>
-    </row>
-    <row r="4" spans="1:15" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="44" t="s">
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="40"/>
+    </row>
+    <row r="4" spans="1:15" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="43" t="s">
         <v>571</v>
       </c>
-      <c r="B4" s="43" t="str">
+      <c r="B4" s="42" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna1]])</f>
         <v>ALEJANDRO EDWARDS</v>
       </c>
-      <c r="C4" s="42" t="str">
+      <c r="C4" s="41" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna2]])</f>
         <v>TAPIA ARAVENA</v>
       </c>
-      <c r="D4" s="36" t="str">
+      <c r="D4" s="35" t="str">
         <f t="shared" si="0"/>
         <v>ALEJANDRO EDWARDS TAPIA ARAVENA</v>
       </c>
-      <c r="E4" s="42" t="str">
+      <c r="E4" s="41" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna3]])</f>
         <v>AYUDANTE MONTAJE GT</v>
       </c>
-      <c r="F4" s="38" t="str">
+      <c r="F4" s="37" t="str">
         <f>UPPER(Tabla1[[#This Row],[NOMBRE COMPLETO]])</f>
         <v>ALEJANDRO EDWARDS TAPIA ARAVENA</v>
       </c>
-      <c r="G4" s="38" t="str">
+      <c r="G4" s="37" t="str">
         <f>UPPER(Tabla1[[#This Row],[CARGO ACTUAL]])</f>
         <v>MECANICO DE MONTAJE</v>
       </c>
-      <c r="H4" s="39" t="s">
+      <c r="H4" s="38" t="s">
         <v>498</v>
       </c>
-      <c r="I4" s="39"/>
-      <c r="J4" s="40" t="s">
+      <c r="I4" s="38"/>
+      <c r="J4" s="39" t="s">
         <v>499</v>
       </c>
-      <c r="K4" s="39" t="s">
+      <c r="K4" s="38" t="s">
         <v>500</v>
       </c>
-      <c r="L4" s="39" t="s">
+      <c r="L4" s="38" t="s">
         <v>501</v>
       </c>
-      <c r="M4" s="39" t="s">
+      <c r="M4" s="38" t="s">
         <v>502</v>
       </c>
-      <c r="N4" s="39" t="s">
+      <c r="N4" s="38" t="s">
         <v>503</v>
       </c>
-      <c r="O4" s="41" t="s">
+      <c r="O4" s="40" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="44" t="s">
+    <row r="5" spans="1:15" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="43" t="s">
         <v>571</v>
       </c>
-      <c r="B5" s="37" t="str">
+      <c r="B5" s="36" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna1]])</f>
         <v>ANDRES IGNACIO</v>
       </c>
-      <c r="C5" s="36" t="str">
+      <c r="C5" s="35" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna2]])</f>
         <v>CRUZ REYES</v>
       </c>
-      <c r="D5" s="36" t="str">
+      <c r="D5" s="35" t="str">
         <f>B5&amp; " " &amp;C5</f>
         <v>ANDRES IGNACIO CRUZ REYES</v>
       </c>
-      <c r="E5" s="36" t="str">
+      <c r="E5" s="35" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna3]])</f>
         <v>AYUDANTE MONTAJE GT</v>
       </c>
-      <c r="F5" s="38" t="str">
+      <c r="F5" s="37" t="str">
         <f>UPPER(Tabla1[[#This Row],[NOMBRE COMPLETO]])</f>
         <v>ANDRÉS IGNACIO CRUZ REYES</v>
       </c>
-      <c r="G5" s="38" t="str">
+      <c r="G5" s="37" t="str">
         <f>UPPER(Tabla1[[#This Row],[CARGO ACTUAL]])</f>
         <v>MONTAJISTA GT</v>
       </c>
-      <c r="H5" s="40">
+      <c r="H5" s="39">
         <v>44256</v>
       </c>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40">
+      <c r="I5" s="39"/>
+      <c r="J5" s="39">
         <v>44256</v>
       </c>
-      <c r="K5" s="39">
+      <c r="K5" s="38">
         <v>3.5</v>
       </c>
-      <c r="L5" s="39" t="s">
+      <c r="L5" s="38" t="s">
         <v>507</v>
       </c>
-      <c r="M5" s="39" t="s">
+      <c r="M5" s="38" t="s">
         <v>508</v>
       </c>
-      <c r="N5" s="39" t="s">
+      <c r="N5" s="38" t="s">
         <v>509</v>
       </c>
-      <c r="O5" s="41" t="s">
+      <c r="O5" s="40" t="s">
         <v>510</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="37" t="str">
+      <c r="A6" s="43" t="s">
+        <v>571</v>
+      </c>
+      <c r="B6" s="36" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna1]])</f>
         <v>BRYAN ESTEBAN</v>
       </c>
-      <c r="C6" s="36" t="str">
+      <c r="C6" s="35" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna2]])</f>
         <v>GAJARDO MARAMBIO</v>
       </c>
@@ -6789,11 +6795,11 @@
       <c r="O6" s="25"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="37" t="str">
+      <c r="B7" s="36" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna1]])</f>
         <v>CARLOS GUSTABO</v>
       </c>
-      <c r="C7" s="36" t="str">
+      <c r="C7" s="35" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna2]])</f>
         <v>ALVARADO SOTO</v>
       </c>
@@ -6823,14 +6829,14 @@
       <c r="O7" s="28"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="43" t="s">
         <v>571</v>
       </c>
-      <c r="B8" s="37" t="str">
+      <c r="B8" s="36" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna1]])</f>
         <v>EDUARDO FRANCISCO</v>
       </c>
-      <c r="C8" s="36" t="str">
+      <c r="C8" s="35" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna2]])</f>
         <v>MUÑOZ MORENO</v>
       </c>
@@ -6872,11 +6878,11 @@
       <c r="O8" s="25"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="37" t="str">
+      <c r="B9" s="36" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna1]])</f>
         <v>ERICK GETHE</v>
       </c>
-      <c r="C9" s="36" t="str">
+      <c r="C9" s="35" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna2]])</f>
         <v>FALKENHAGEN CASTILLO</v>
       </c>
@@ -6906,11 +6912,11 @@
       <c r="O9" s="28"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="37" t="str">
+      <c r="B10" s="36" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna1]])</f>
         <v>FABIAN ALEJANDRO</v>
       </c>
-      <c r="C10" s="36" t="str">
+      <c r="C10" s="35" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna2]])</f>
         <v>VARAS MUÑOZ</v>
       </c>
@@ -6954,11 +6960,11 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="37" t="str">
+      <c r="B11" s="36" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna1]])</f>
         <v>FELIPE EDUARDO</v>
       </c>
-      <c r="C11" s="36" t="str">
+      <c r="C11" s="35" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna2]])</f>
         <v>ARRIAGADA HERRERA</v>
       </c>
@@ -6988,11 +6994,11 @@
       <c r="O11" s="28"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="37" t="str">
+      <c r="B12" s="36" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna1]])</f>
         <v>FRANCISCO JAVIER</v>
       </c>
-      <c r="C12" s="36" t="str">
+      <c r="C12" s="35" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna2]])</f>
         <v>ESPARZA RIQUELME</v>
       </c>
@@ -7022,11 +7028,11 @@
       <c r="O12" s="25"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="37" t="str">
+      <c r="B13" s="36" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna1]])</f>
         <v>FRANCO ESTEBAN</v>
       </c>
-      <c r="C13" s="36" t="str">
+      <c r="C13" s="35" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna2]])</f>
         <v>GONZALEZ TORO</v>
       </c>
@@ -7056,11 +7062,11 @@
       <c r="O13" s="28"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="37" t="str">
+      <c r="B14" s="36" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna1]])</f>
         <v>GEORGE ADRIAN</v>
       </c>
-      <c r="C14" s="36" t="str">
+      <c r="C14" s="35" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna2]])</f>
         <v>CARRASCO VEGA</v>
       </c>
@@ -7090,11 +7096,11 @@
       <c r="O14" s="25"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="37" t="str">
+      <c r="B15" s="36" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna1]])</f>
         <v>GONZALO ANDRÉS</v>
       </c>
-      <c r="C15" s="36" t="str">
+      <c r="C15" s="35" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna2]])</f>
         <v>VALDÉZ VALDÉZ</v>
       </c>
@@ -7138,11 +7144,11 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="37" t="str">
+      <c r="B16" s="36" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna1]])</f>
         <v>HECTOR ANDRES</v>
       </c>
-      <c r="C16" s="36" t="str">
+      <c r="C16" s="35" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna2]])</f>
         <v>MERA AVELLO</v>
       </c>
@@ -7172,11 +7178,11 @@
       <c r="O16" s="25"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="37" t="str">
+      <c r="B17" s="36" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna1]])</f>
         <v>JOAQUIN IGNACIO</v>
       </c>
-      <c r="C17" s="36" t="str">
+      <c r="C17" s="35" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna2]])</f>
         <v>GONZALEZ ASTORGA</v>
       </c>
@@ -7220,11 +7226,11 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="37" t="str">
+      <c r="B18" s="36" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna1]])</f>
         <v>JORGE GABRIEL</v>
       </c>
-      <c r="C18" s="36" t="str">
+      <c r="C18" s="35" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna2]])</f>
         <v>PEREZ VELÁSQUEZ</v>
       </c>
@@ -7254,11 +7260,11 @@
       <c r="O18" s="25"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="37" t="str">
+      <c r="B19" s="36" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna1]])</f>
         <v>JOVANY FRANCISCO</v>
       </c>
-      <c r="C19" s="36" t="str">
+      <c r="C19" s="35" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna2]])</f>
         <v>ROJAS HERRERA</v>
       </c>
@@ -7288,14 +7294,14 @@
       <c r="O19" s="28"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="44" t="s">
+      <c r="A20" s="43" t="s">
         <v>571</v>
       </c>
-      <c r="B20" s="37" t="str">
+      <c r="B20" s="36" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna1]])</f>
         <v>LEONARDO FELICIANO</v>
       </c>
-      <c r="C20" s="36" t="str">
+      <c r="C20" s="35" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna2]])</f>
         <v>OSORIO CATRILAF</v>
       </c>
@@ -7325,11 +7331,11 @@
       <c r="O20" s="25"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="37" t="str">
+      <c r="B21" s="36" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna1]])</f>
         <v>LUIS FERNANDO</v>
       </c>
-      <c r="C21" s="36" t="str">
+      <c r="C21" s="35" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna2]])</f>
         <v>ORTIZ GUTIERREZ</v>
       </c>
@@ -7359,14 +7365,14 @@
       <c r="O21" s="28"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="43" t="s">
         <v>571</v>
       </c>
-      <c r="B22" s="37" t="str">
+      <c r="B22" s="36" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna1]])</f>
         <v>MARIO ALFREDO</v>
       </c>
-      <c r="C22" s="36" t="str">
+      <c r="C22" s="35" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna2]])</f>
         <v>VERGARA PEREZ</v>
       </c>
@@ -7396,11 +7402,11 @@
       <c r="O22" s="25"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="37" t="str">
+      <c r="B23" s="36" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna1]])</f>
         <v>MATIAS FELIPE</v>
       </c>
-      <c r="C23" s="36" t="str">
+      <c r="C23" s="35" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna2]])</f>
         <v>GONZALEZ SILVA</v>
       </c>
@@ -7444,11 +7450,11 @@
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B24" s="37" t="str">
+      <c r="B24" s="36" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna1]])</f>
         <v>PATRICIO ALBERTO</v>
       </c>
-      <c r="C24" s="36" t="str">
+      <c r="C24" s="35" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna2]])</f>
         <v>FERNANDEZ GONZALEZ</v>
       </c>
@@ -7492,11 +7498,11 @@
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="37" t="str">
+      <c r="B25" s="36" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna1]])</f>
         <v>RICARDO ANDRÉS</v>
       </c>
-      <c r="C25" s="36" t="str">
+      <c r="C25" s="35" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna2]])</f>
         <v>LEAL TAPIA</v>
       </c>
@@ -7540,11 +7546,11 @@
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="37" t="str">
+      <c r="B26" s="36" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna1]])</f>
         <v>ROGELIO ANTONIO</v>
       </c>
-      <c r="C26" s="36" t="str">
+      <c r="C26" s="35" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna2]])</f>
         <v>MELLA PERALTA</v>
       </c>
@@ -7588,11 +7594,11 @@
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B27" s="37" t="str">
+      <c r="B27" s="36" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna1]])</f>
         <v>SEBASTIAN ANDRES</v>
       </c>
-      <c r="C27" s="36" t="str">
+      <c r="C27" s="35" t="str">
         <f>UPPER(Tabla33[[#This Row],[Columna2]])</f>
         <v>VALENZUELA ENSEMEYER</v>
       </c>
@@ -7642,12 +7648,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7783,15 +7786,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C943B3BD-8BE8-47E1-B812-F13C36219531}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8233E96-18B0-4EBC-8430-25DA7C336409}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="2aab30d0-8d3a-4111-bc7a-be1762f05546"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7815,17 +7829,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8233E96-18B0-4EBC-8430-25DA7C336409}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C943B3BD-8BE8-47E1-B812-F13C36219531}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="2aab30d0-8d3a-4111-bc7a-be1762f05546"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>